<commit_message>
Change consumer monitoring to Consumption Monitoring
</commit_message>
<xml_diff>
--- a/TimeSheet/Content/Dash_Board.xlsx
+++ b/TimeSheet/Content/Dash_Board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="-30" windowWidth="2760" windowHeight="4710" tabRatio="841" firstSheet="1" activeTab="1"/>
@@ -347,9 +347,6 @@
     <t xml:space="preserve">Compliance driven projects / programs </t>
   </si>
   <si>
-    <t>comsumer monitoring (test supported)</t>
-  </si>
-  <si>
     <t>Baby-Feminine-Fam care</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t xml:space="preserve">Claims/Copy Support </t>
   </si>
   <si>
-    <t xml:space="preserve">comsumer monitoring </t>
-  </si>
-  <si>
     <t>TARGET / COMNMENTS</t>
   </si>
   <si>
@@ -441,6 +435,12 @@
   </si>
   <si>
     <t>Updated: 25-Sept-2013</t>
+  </si>
+  <si>
+    <t>consumer monitoring (test supported)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumer monitoring </t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1440,7 @@
     <row r="1" spans="1:1">
       <c r="A1">
         <f ca="1">NOW()</f>
-        <v>41698.575901504628</v>
+        <v>41698.665745833336</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1451,7 +1451,7 @@
     <row r="5" spans="1:1">
       <c r="A5">
         <f ca="1">NOW()</f>
-        <v>41698.575901504628</v>
+        <v>41698.665745833336</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -1472,7 +1472,7 @@
   </sheetPr>
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C35" sqref="C35:C42"/>
     </sheetView>
   </sheetViews>
@@ -1501,7 +1501,7 @@
       <c r="B1" s="8"/>
       <c r="E1" s="41"/>
       <c r="I1" s="101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="C4" s="78"/>
       <c r="D4" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="47"/>
       <c r="G4" s="27" t="s">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="87"/>
     </row>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -1584,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="64"/>
     </row>
@@ -1595,7 +1595,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="89"/>
@@ -1609,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="64"/>
       <c r="P10" s="2"/>
@@ -1622,7 +1622,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="90"/>
@@ -1664,7 +1664,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>51</v>
@@ -1673,7 +1673,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1710,7 +1710,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="102"/>
       <c r="D17" s="7"/>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="102"/>
       <c r="D18" s="7"/>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="102"/>
       <c r="D19" s="7"/>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="7"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
@@ -1815,31 +1815,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -1876,7 +1876,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="102"/>
       <c r="D27" s="102"/>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="102"/>
       <c r="D28" s="102"/>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="102"/>
       <c r="D29" s="102"/>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="31" spans="2:13" ht="24.75" customHeight="1">
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="106"/>
       <c r="D31" s="102"/>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="107" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="108"/>
       <c r="D33" s="108"/>
@@ -1985,31 +1985,31 @@
         <v>3</v>
       </c>
       <c r="D34" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -2058,7 +2058,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="102"/>
       <c r="D38" s="7"/>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="7"/>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="106"/>
       <c r="D40" s="7"/>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="42" spans="2:16" ht="24" customHeight="1">
       <c r="B42" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="106"/>
       <c r="D42" s="7"/>
@@ -2208,7 +2208,7 @@
       <c r="E46" s="113"/>
       <c r="F46" s="114"/>
       <c r="G46" s="109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="110"/>
@@ -2430,30 +2430,30 @@
     </row>
     <row r="60" spans="2:16" s="29" customFormat="1" ht="69" customHeight="1">
       <c r="B60" s="98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="99"/>
       <c r="F60" s="98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I60" s="99"/>
       <c r="J60" s="99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K60" s="98"/>
       <c r="L60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N60" s="53"/>
       <c r="O60" s="54"/>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="68" spans="2:10">
       <c r="B68" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="100">
         <v>1</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="75" spans="2:10" s="48" customFormat="1">
       <c r="B75" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="70"/>
       <c r="D75" s="70"/>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="76" spans="2:10" ht="22.5" customHeight="1">
       <c r="B76" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -2687,7 +2687,7 @@
       <c r="B1" s="8"/>
       <c r="E1" s="41"/>
       <c r="I1" s="101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="C4" s="78"/>
       <c r="D4" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="47"/>
       <c r="G4" s="27" t="s">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="87"/>
     </row>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -2770,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="64"/>
     </row>
@@ -2781,7 +2781,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="89"/>
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="64"/>
       <c r="P10" s="23"/>
@@ -2808,7 +2808,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="90"/>
@@ -2850,7 +2850,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>51</v>
@@ -2859,7 +2859,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2896,7 +2896,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="102"/>
       <c r="D17" s="102"/>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="102"/>
       <c r="D18" s="102"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="102"/>
       <c r="D19" s="102"/>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="102"/>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
@@ -3001,31 +3001,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -3062,7 +3062,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="102"/>
       <c r="D27" s="102"/>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="102"/>
       <c r="D28" s="102"/>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="102"/>
       <c r="D29" s="102"/>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="106"/>
       <c r="D31" s="102"/>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="107" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="108"/>
       <c r="D33" s="108"/>
@@ -3171,31 +3171,31 @@
         <v>3</v>
       </c>
       <c r="D34" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -3244,7 +3244,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="102"/>
       <c r="D38" s="102"/>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="102"/>
@@ -3276,7 +3276,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="106"/>
       <c r="D40" s="102"/>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="42" spans="2:16" ht="24" customHeight="1">
       <c r="B42" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="106"/>
       <c r="D42" s="102"/>
@@ -3394,7 +3394,7 @@
       <c r="E46" s="113"/>
       <c r="F46" s="114"/>
       <c r="G46" s="109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="110"/>
@@ -3616,30 +3616,30 @@
     </row>
     <row r="60" spans="2:16" s="29" customFormat="1" ht="69" customHeight="1">
       <c r="B60" s="98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="99"/>
       <c r="F60" s="98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I60" s="99"/>
       <c r="J60" s="99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K60" s="98"/>
       <c r="L60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N60" s="53"/>
       <c r="O60" s="54"/>
@@ -3718,7 +3718,7 @@
     </row>
     <row r="68" spans="2:10">
       <c r="B68" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -3784,7 +3784,7 @@
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="100">
         <v>1</v>
@@ -3803,7 +3803,7 @@
     </row>
     <row r="75" spans="2:10" s="48" customFormat="1">
       <c r="B75" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="70"/>
       <c r="D75" s="70"/>
@@ -3814,7 +3814,7 @@
     </row>
     <row r="76" spans="2:10">
       <c r="B76" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -3871,7 +3871,7 @@
       <c r="B1" s="8"/>
       <c r="E1" s="41"/>
       <c r="I1" s="101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="C4" s="78"/>
       <c r="D4" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="47"/>
       <c r="G4" s="27" t="s">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="87"/>
     </row>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -3954,7 +3954,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="64"/>
     </row>
@@ -3965,7 +3965,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="89"/>
@@ -3979,7 +3979,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="64"/>
       <c r="P10" s="23"/>
@@ -3992,7 +3992,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="90"/>
@@ -4034,7 +4034,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>51</v>
@@ -4043,7 +4043,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -4080,7 +4080,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="7"/>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
@@ -4185,31 +4185,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -4246,7 +4246,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="7"/>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="107" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="108"/>
       <c r="D33" s="108"/>
@@ -4355,31 +4355,31 @@
         <v>3</v>
       </c>
       <c r="D34" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -4428,7 +4428,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
@@ -4460,7 +4460,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="7"/>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="42" spans="2:16" ht="24" customHeight="1">
       <c r="B42" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="7"/>
@@ -4578,7 +4578,7 @@
       <c r="E46" s="113"/>
       <c r="F46" s="114"/>
       <c r="G46" s="109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="110"/>
@@ -4800,30 +4800,30 @@
     </row>
     <row r="60" spans="2:16" s="29" customFormat="1" ht="69" customHeight="1">
       <c r="B60" s="98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="99"/>
       <c r="F60" s="98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I60" s="99"/>
       <c r="J60" s="99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K60" s="98"/>
       <c r="L60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N60" s="53"/>
       <c r="O60" s="54"/>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="68" spans="2:10">
       <c r="B68" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -4968,7 +4968,7 @@
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="100">
         <v>1</v>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="75" spans="2:10" s="48" customFormat="1">
       <c r="B75" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="70"/>
       <c r="D75" s="70"/>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="76" spans="2:10">
       <c r="B76" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -5055,7 +5055,7 @@
       <c r="B1" s="8"/>
       <c r="E1" s="41"/>
       <c r="I1" s="101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75">
@@ -5089,7 +5089,7 @@
       </c>
       <c r="C4" s="78"/>
       <c r="D4" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="47"/>
       <c r="G4" s="27" t="s">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="87"/>
     </row>
@@ -5127,7 +5127,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -5138,7 +5138,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="64"/>
     </row>
@@ -5149,7 +5149,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="89"/>
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="64"/>
       <c r="P10" s="23"/>
@@ -5176,7 +5176,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="90"/>
@@ -5218,7 +5218,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>51</v>
@@ -5227,7 +5227,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5264,7 +5264,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="102"/>
       <c r="D17" s="102"/>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="102"/>
       <c r="D18" s="102"/>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="102"/>
       <c r="D19" s="102"/>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="102"/>
@@ -5354,7 +5354,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
@@ -5369,31 +5369,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -5430,7 +5430,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="102"/>
       <c r="D27" s="102"/>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="102"/>
       <c r="D28" s="102"/>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="102"/>
       <c r="D29" s="102"/>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="106"/>
       <c r="D31" s="102"/>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="107" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="108"/>
       <c r="D33" s="108"/>
@@ -5539,31 +5539,31 @@
         <v>3</v>
       </c>
       <c r="D34" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -5612,7 +5612,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="102"/>
       <c r="D38" s="102"/>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="102"/>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="106"/>
       <c r="D40" s="102"/>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="42" spans="2:16" ht="24" customHeight="1">
       <c r="B42" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="106"/>
       <c r="D42" s="102"/>
@@ -5762,7 +5762,7 @@
       <c r="E46" s="113"/>
       <c r="F46" s="114"/>
       <c r="G46" s="109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="110"/>
@@ -5984,30 +5984,30 @@
     </row>
     <row r="60" spans="2:16" s="29" customFormat="1" ht="69" customHeight="1">
       <c r="B60" s="98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="99"/>
       <c r="F60" s="98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I60" s="99"/>
       <c r="J60" s="99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K60" s="98"/>
       <c r="L60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N60" s="53"/>
       <c r="O60" s="54"/>
@@ -6086,7 +6086,7 @@
     </row>
     <row r="68" spans="2:10">
       <c r="B68" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -6152,7 +6152,7 @@
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="100">
         <v>1</v>
@@ -6171,7 +6171,7 @@
     </row>
     <row r="75" spans="2:10" s="48" customFormat="1">
       <c r="B75" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="70"/>
       <c r="D75" s="70"/>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="76" spans="2:10">
       <c r="B76" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -6239,7 +6239,7 @@
       <c r="B1" s="8"/>
       <c r="E1" s="41"/>
       <c r="I1" s="101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="C4" s="78"/>
       <c r="D4" s="85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="47"/>
       <c r="G4" s="27" t="s">
@@ -6281,7 +6281,7 @@
       </c>
       <c r="H4" s="27"/>
       <c r="I4" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="87"/>
     </row>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -6322,7 +6322,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="64"/>
     </row>
@@ -6333,7 +6333,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="89"/>
@@ -6347,7 +6347,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="64"/>
       <c r="P10" s="23"/>
@@ -6360,7 +6360,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="90"/>
@@ -6402,7 +6402,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>51</v>
@@ -6411,7 +6411,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -6448,7 +6448,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="102"/>
       <c r="D17" s="102"/>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="102"/>
       <c r="D18" s="102"/>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="102"/>
       <c r="D19" s="102"/>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="102"/>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
@@ -6553,31 +6553,31 @@
         <v>3</v>
       </c>
       <c r="D24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -6614,7 +6614,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="102"/>
       <c r="D27" s="102"/>
@@ -6630,7 +6630,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="102"/>
       <c r="D28" s="102"/>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="102"/>
       <c r="D29" s="102"/>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="106"/>
       <c r="D31" s="102"/>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="107" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="108"/>
       <c r="D33" s="108"/>
@@ -6723,31 +6723,31 @@
         <v>3</v>
       </c>
       <c r="D34" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>51</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -6796,7 +6796,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="102"/>
       <c r="D38" s="102"/>
@@ -6812,7 +6812,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="102"/>
@@ -6828,7 +6828,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="106"/>
       <c r="D40" s="102"/>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="42" spans="2:16" ht="24" customHeight="1">
       <c r="B42" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="106"/>
       <c r="D42" s="102"/>
@@ -6946,7 +6946,7 @@
       <c r="E46" s="113"/>
       <c r="F46" s="114"/>
       <c r="G46" s="109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="110"/>
@@ -7168,30 +7168,30 @@
     </row>
     <row r="60" spans="2:16" s="29" customFormat="1" ht="69" customHeight="1">
       <c r="B60" s="98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="98"/>
       <c r="D60" s="98"/>
       <c r="E60" s="99"/>
       <c r="F60" s="98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I60" s="99"/>
       <c r="J60" s="99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K60" s="98"/>
       <c r="L60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M60" s="99" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N60" s="53"/>
       <c r="O60" s="54"/>
@@ -7270,7 +7270,7 @@
     </row>
     <row r="68" spans="2:10">
       <c r="B68" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" s="100">
         <v>1</v>
@@ -7355,7 +7355,7 @@
     </row>
     <row r="75" spans="2:10" s="48" customFormat="1">
       <c r="B75" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="70"/>
       <c r="D75" s="70"/>
@@ -7366,7 +7366,7 @@
     </row>
     <row r="76" spans="2:10">
       <c r="B76" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -7391,12 +7391,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7449,15 +7446,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4860FA-6862-47CF-82FB-EE89C1981EA8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32C936E8-4A99-4EBD-BA5A-FB2A1938ED8E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7478,9 +7478,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32C936E8-4A99-4EBD-BA5A-FB2A1938ED8E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4860FA-6862-47CF-82FB-EE89C1981EA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>